<commit_message>
removed duplicate query from test set (#9 & #10)
</commit_message>
<xml_diff>
--- a/analysis_lubm100.xlsx
+++ b/analysis_lubm100.xlsx
@@ -4,17 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="19155" windowHeight="12525"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="19155" windowHeight="12465" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="stardog_lubm100" sheetId="1" r:id="rId1"/>
-    <sheet name="log-oracle-tz_18M_CDM" sheetId="3" r:id="rId2"/>
-    <sheet name="log-stardog_18M_CDM" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="virtuoso_lubm100" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="log" localSheetId="1">'log-oracle-tz_18M_CDM'!$A$2:$D$61</definedName>
-    <definedName name="log" localSheetId="2">'log-stardog_18M_CDM'!$A$2:$D$61</definedName>
+    <definedName name="log" localSheetId="1">virtuoso_lubm100!$A$2:$D$61</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -32,21 +30,11 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="log1" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="D:\git\cdm_test_suite\stardog\log.csv" tab="0" comma="1">
-      <textFields count="4">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>iteration</t>
   </si>
@@ -58,9 +46,6 @@
   </si>
   <si>
     <t>retrieved results</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>average response time</t>
@@ -633,13 +618,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Average</a:t>
+              <a:t>Average Response Time</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Response Time</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -670,100 +650,110 @@
             <c:v>virtuoso</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>stardog_lubm100!$I$2:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stardog_lubm100!$J$2:$J$13</c:f>
+              <c:f>virtuoso_lubm100!$J$2:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.2399999999999998</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2459999999999996</c:v>
+                  <c:v>4.0340000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>1.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17800000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>260.97200000000004</c:v>
+                  <c:v>5.4139999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.982</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9579999999999997</c:v>
+                  <c:v>5.5819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0880000000000001</c:v>
+                  <c:v>5.55</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.73</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.53</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.2000000000000012E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>oracle</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'log-oracle-tz_18M_CDM'!$J$2:$J$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.80199999999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.8200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>153.16999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24.201999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300.202</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>300.32799999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>160.82799999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>163.39000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.972</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.16599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>162.96800000000002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>17.566000000000003</c:v>
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.6659999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -771,52 +761,115 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>stardog</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>stardog_lubm100!$I$2:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log-stardog_18M_CDM'!$J$2:$J$13</c:f>
+              <c:f>stardog_lubm100!$J$2:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.0640000000000001</c:v>
+                  <c:v>1.2399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64399999999999991</c:v>
+                  <c:v>7.2459999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.944</c:v>
+                  <c:v>3.2000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10200000000000001</c:v>
+                  <c:v>0.17800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>203.57599999999996</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>168.29</c:v>
+                  <c:v>260.97200000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.38</c:v>
+                  <c:v>1.982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1</c:v>
+                  <c:v>2.9579999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.20400000000000001</c:v>
+                  <c:v>3.0880000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19399999999999998</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.22000000000000003</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.818000000000001</c:v>
+                  <c:v>9.2000000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8980000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -841,6 +894,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -877,6 +931,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr u="none"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -946,12 +1010,66 @@
             <c:v>virtuoso</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>stardog_lubm100!$I$2:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stardog_lubm100!$K$2:$K$13</c:f>
+              <c:f>virtuoso_lubm100!$K$2:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -962,31 +1080,40 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>719</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7790</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>27247</c:v>
+                  <c:v>13200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,103 +1123,113 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>oracle</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'log-oracle-tz_18M_CDM'!$K$2:$K$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14848</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24701</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24701</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>759</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3485</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
             <c:v>stardog</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>stardog_lubm100!$I$2:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log-stardog_18M_CDM'!$K$2:$K$13</c:f>
+              <c:f>stardog_lubm100!$K$2:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14610</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>348</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>719</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2647</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2647</c:v>
+                  <c:v>7790</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>27247</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3437</c:v>
+                <c:pt idx="14">
+                  <c:v>795970</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1117,6 +1254,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1230,10 +1368,6 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="log" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="log" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1525,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -2772,10 +2906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K9"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2805,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -2819,21 +2953,21 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.64</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
         <f>AVERAGE(C2:C6)</f>
-        <v>0.80199999999999994</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="K2">
         <f>LOOKUP(I2,B:B,D:D)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2844,21 +2978,21 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
         <f>AVERAGE(C7:C11)</f>
-        <v>3.8200000000000003</v>
+        <v>4.0340000000000007</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K13" si="0">LOOKUP(I3,B:B,D:D)</f>
-        <v>14848</v>
+        <f t="shared" ref="K3:K16" si="0">LOOKUP(I3,B:B,D:D)</f>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2869,21 +3003,21 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4">
         <f>AVERAGE(C12:C16)</f>
-        <v>153.16999999999999</v>
+        <v>1.67</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2894,21 +3028,21 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.09</v>
+        <v>0.01</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
       <c r="J5">
         <f>AVERAGE(C17:C21)</f>
-        <v>24.201999999999998</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2919,21 +3053,21 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6">
         <f>AVERAGE(C22:C26)</f>
-        <v>300.202</v>
-      </c>
-      <c r="K6" s="1" t="str">
+        <v>0.01</v>
+      </c>
+      <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>N/A</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2944,21 +3078,21 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3.71</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="D7">
-        <v>14848</v>
+        <v>264</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7">
         <f>AVERAGE(C27:C31)</f>
-        <v>300.32799999999997</v>
-      </c>
-      <c r="K7" s="1" t="str">
+        <v>5.4139999999999997</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>N/A</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2969,21 +3103,21 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>4.08</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>14848</v>
+        <v>264</v>
       </c>
       <c r="I8">
         <v>6</v>
       </c>
       <c r="J8">
         <f>AVERAGE(C32:C36)</f>
-        <v>160.82799999999997</v>
+        <v>0.01</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>24701</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2994,21 +3128,21 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>3.79</v>
+        <v>4.01</v>
       </c>
       <c r="D9">
-        <v>14848</v>
+        <v>264</v>
       </c>
       <c r="I9">
         <v>7</v>
       </c>
       <c r="J9">
         <f>AVERAGE(C37:C41)</f>
-        <v>163.39000000000001</v>
+        <v>5.5819999999999999</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>24701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3019,21 +3153,21 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>3.65</v>
+        <v>4.07</v>
       </c>
       <c r="D10">
-        <v>14848</v>
+        <v>264</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
       <c r="J10">
         <f>AVERAGE(C42:C46)</f>
-        <v>3.972</v>
+        <v>5.55</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3044,21 +3178,21 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>3.87</v>
+        <v>4.03</v>
       </c>
       <c r="D11">
-        <v>14848</v>
+        <v>264</v>
       </c>
       <c r="I11">
         <v>9</v>
       </c>
       <c r="J11">
         <f>AVERAGE(C47:C51)</f>
-        <v>0.16599999999999998</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3069,21 +3203,21 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>148.63999999999999</v>
+        <v>1.67</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12">
         <f>AVERAGE(C52:C56)</f>
-        <v>162.96800000000002</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3094,21 +3228,21 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>157.29</v>
+        <v>1.67</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I13">
         <v>11</v>
       </c>
       <c r="J13">
         <f>AVERAGE(C57:C61)</f>
-        <v>17.566000000000003</v>
+        <v>0.01</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>3485</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3119,10 +3253,21 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>148.9</v>
+        <v>1.67</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <f>AVERAGE(C62:C66)</f>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3133,10 +3278,21 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>153.5</v>
+        <v>1.67</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>13</v>
+      </c>
+      <c r="J15">
+        <f>AVERAGE(C67:C71)</f>
+        <v>0.01</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3147,10 +3303,21 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>157.52000000000001</v>
+        <v>1.67</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(C72:C76)</f>
+        <v>5.6659999999999995</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>100000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,10 +3328,10 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>21.98</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3175,10 +3342,10 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>25.69</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,10 +3356,10 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>22.02</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3203,10 +3370,10 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>30.08</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3217,10 +3384,10 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>21.24</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3231,10 +3398,10 @@
         <v>4</v>
       </c>
       <c r="C22">
-        <v>300.19</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
+        <v>0.01</v>
+      </c>
+      <c r="D22">
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3245,10 +3412,10 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>300.14999999999998</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
+        <v>0.01</v>
+      </c>
+      <c r="D23">
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3259,10 +3426,10 @@
         <v>4</v>
       </c>
       <c r="C24">
-        <v>300.17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
+        <v>0.01</v>
+      </c>
+      <c r="D24">
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3273,10 +3440,10 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>300.18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
+        <v>0.01</v>
+      </c>
+      <c r="D25">
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,10 +3454,10 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>300.32</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
+        <v>0.01</v>
+      </c>
+      <c r="D26">
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,10 +3468,10 @@
         <v>5</v>
       </c>
       <c r="C27">
-        <v>300.33999999999997</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
+        <v>5.41</v>
+      </c>
+      <c r="D27">
+        <v>100000</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,10 +3482,10 @@
         <v>5</v>
       </c>
       <c r="C28">
-        <v>300.3</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
+        <v>5.41</v>
+      </c>
+      <c r="D28">
+        <v>100000</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3329,10 +3496,10 @@
         <v>5</v>
       </c>
       <c r="C29">
-        <v>300.32</v>
-      </c>
-      <c r="D29" t="s">
-        <v>4</v>
+        <v>5.42</v>
+      </c>
+      <c r="D29">
+        <v>100000</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3343,10 +3510,10 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>300.33999999999997</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4</v>
+        <v>5.4</v>
+      </c>
+      <c r="D30">
+        <v>100000</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3357,10 +3524,10 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>300.33999999999997</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4</v>
+        <v>5.43</v>
+      </c>
+      <c r="D31">
+        <v>100000</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3371,10 +3538,10 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>157.97</v>
+        <v>0.01</v>
       </c>
       <c r="D32">
-        <v>24701</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3385,10 +3552,10 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>157.44999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="D33">
-        <v>24701</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3399,10 +3566,10 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>153.99</v>
+        <v>0.01</v>
       </c>
       <c r="D34">
-        <v>24701</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3413,10 +3580,10 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>161.66999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="D35">
-        <v>24701</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3427,10 +3594,10 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>173.06</v>
+        <v>0.01</v>
       </c>
       <c r="D36">
-        <v>24701</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3441,10 +3608,10 @@
         <v>7</v>
       </c>
       <c r="C37">
-        <v>169.2</v>
+        <v>5.59</v>
       </c>
       <c r="D37">
-        <v>24701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3455,10 +3622,10 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <v>165.77</v>
+        <v>5.5</v>
       </c>
       <c r="D38">
-        <v>24701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3469,10 +3636,10 @@
         <v>7</v>
       </c>
       <c r="C39">
-        <v>150.38999999999999</v>
+        <v>5.63</v>
       </c>
       <c r="D39">
-        <v>24701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3483,10 +3650,10 @@
         <v>7</v>
       </c>
       <c r="C40">
-        <v>180.64</v>
+        <v>5.6</v>
       </c>
       <c r="D40">
-        <v>24701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3497,10 +3664,10 @@
         <v>7</v>
       </c>
       <c r="C41">
-        <v>150.94999999999999</v>
+        <v>5.59</v>
       </c>
       <c r="D41">
-        <v>24701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3511,10 +3678,10 @@
         <v>8</v>
       </c>
       <c r="C42">
-        <v>4.0199999999999996</v>
+        <v>5.54</v>
       </c>
       <c r="D42">
-        <v>70</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3525,10 +3692,10 @@
         <v>8</v>
       </c>
       <c r="C43">
-        <v>3.88</v>
+        <v>5.54</v>
       </c>
       <c r="D43">
-        <v>70</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,10 +3706,10 @@
         <v>8</v>
       </c>
       <c r="C44">
-        <v>3.97</v>
+        <v>5.53</v>
       </c>
       <c r="D44">
-        <v>70</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3553,10 +3720,10 @@
         <v>8</v>
       </c>
       <c r="C45">
-        <v>3.98</v>
+        <v>5.54</v>
       </c>
       <c r="D45">
-        <v>70</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3567,10 +3734,10 @@
         <v>8</v>
       </c>
       <c r="C46">
-        <v>4.01</v>
+        <v>5.6</v>
       </c>
       <c r="D46">
-        <v>70</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3581,10 +3748,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3595,10 +3762,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3609,10 +3776,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,10 +3790,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3637,10 +3804,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3651,10 +3818,10 @@
         <v>10</v>
       </c>
       <c r="C52">
-        <v>300.33</v>
-      </c>
-      <c r="D52" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,10 +3832,10 @@
         <v>10</v>
       </c>
       <c r="C53">
-        <v>300.35000000000002</v>
-      </c>
-      <c r="D53" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3679,10 +3846,10 @@
         <v>10</v>
       </c>
       <c r="C54">
-        <v>147.79</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3693,10 +3860,10 @@
         <v>10</v>
       </c>
       <c r="C55">
-        <v>27.08</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,10 +3874,10 @@
         <v>10</v>
       </c>
       <c r="C56">
-        <v>39.29</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3721,10 +3888,10 @@
         <v>11</v>
       </c>
       <c r="C57">
-        <v>20.12</v>
+        <v>0.01</v>
       </c>
       <c r="D57">
-        <v>3485</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3735,10 +3902,10 @@
         <v>11</v>
       </c>
       <c r="C58">
-        <v>15.64</v>
+        <v>0.01</v>
       </c>
       <c r="D58">
-        <v>3485</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,10 +3916,10 @@
         <v>11</v>
       </c>
       <c r="C59">
-        <v>14.61</v>
+        <v>0.01</v>
       </c>
       <c r="D59">
-        <v>3485</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3763,10 +3930,10 @@
         <v>11</v>
       </c>
       <c r="C60">
-        <v>14.87</v>
+        <v>0.01</v>
       </c>
       <c r="D60">
-        <v>3485</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,10 +3944,220 @@
         <v>11</v>
       </c>
       <c r="C61">
-        <v>22.59</v>
+        <v>0.01</v>
       </c>
       <c r="D61">
-        <v>3485</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>0.32</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64">
+        <v>12</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>12</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66">
+        <v>12</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>13</v>
+      </c>
+      <c r="C67">
+        <v>0.01</v>
+      </c>
+      <c r="D67">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <v>0.01</v>
+      </c>
+      <c r="D68">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69">
+        <v>13</v>
+      </c>
+      <c r="C69">
+        <v>0.01</v>
+      </c>
+      <c r="D69">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>13</v>
+      </c>
+      <c r="C70">
+        <v>0.01</v>
+      </c>
+      <c r="D70">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>4</v>
+      </c>
+      <c r="B71">
+        <v>13</v>
+      </c>
+      <c r="C71">
+        <v>0.01</v>
+      </c>
+      <c r="D71">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>5.62</v>
+      </c>
+      <c r="D72">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>5.68</v>
+      </c>
+      <c r="D73">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>14</v>
+      </c>
+      <c r="C74">
+        <v>5.67</v>
+      </c>
+      <c r="D74">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <v>5.69</v>
+      </c>
+      <c r="D75">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>4</v>
+      </c>
+      <c r="B76">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <v>5.67</v>
+      </c>
+      <c r="D76">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -3793,1032 +4170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K61"/>
-  <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1.51</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f>AVERAGE(C2:C6)</f>
-        <v>1.0640000000000001</v>
-      </c>
-      <c r="K2">
-        <f>LOOKUP(I2,B:B,D:D)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0.91</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <f>AVERAGE(C7:C11)</f>
-        <v>0.64399999999999991</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K13" si="0">LOOKUP(I3,B:B,D:D)</f>
-        <v>14610</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0.94</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <f>AVERAGE(C12:C16)</f>
-        <v>2.944</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1.01</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <f>AVERAGE(C17:C21)</f>
-        <v>0.10200000000000001</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>348</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0.95</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <f>AVERAGE(C22:C26)</f>
-        <v>203.57599999999996</v>
-      </c>
-      <c r="K6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1.82</v>
-      </c>
-      <c r="D7">
-        <v>14610</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <f>AVERAGE(C27:C31)</f>
-        <v>168.29</v>
-      </c>
-      <c r="K7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0.36</v>
-      </c>
-      <c r="D8">
-        <v>14610</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8">
-        <f>AVERAGE(C32:C36)</f>
-        <v>2.38</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0.34</v>
-      </c>
-      <c r="D9">
-        <v>14610</v>
-      </c>
-      <c r="I9">
-        <v>7</v>
-      </c>
-      <c r="J9">
-        <f>AVERAGE(C37:C41)</f>
-        <v>2.1</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0.36</v>
-      </c>
-      <c r="D10">
-        <v>14610</v>
-      </c>
-      <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10">
-        <f>AVERAGE(C42:C46)</f>
-        <v>0.20400000000000001</v>
-      </c>
-      <c r="K10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0.34</v>
-      </c>
-      <c r="D11">
-        <v>14610</v>
-      </c>
-      <c r="I11">
-        <v>9</v>
-      </c>
-      <c r="J11">
-        <f>AVERAGE(C47:C51)</f>
-        <v>0.19399999999999998</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>4.66</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>10</v>
-      </c>
-      <c r="J12">
-        <f>AVERAGE(C52:C56)</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>696</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2.48</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <v>11</v>
-      </c>
-      <c r="J13">
-        <f>AVERAGE(C57:C61)</f>
-        <v>10.818000000000001</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>2.54</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>2.5</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>2.54</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>0.27</v>
-      </c>
-      <c r="D17">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>0.06</v>
-      </c>
-      <c r="D18">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>0.06</v>
-      </c>
-      <c r="D19">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>0.06</v>
-      </c>
-      <c r="D20">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>0.06</v>
-      </c>
-      <c r="D21">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>300.29000000000002</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23">
-        <v>175.45</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>177.66</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25">
-        <v>177.53</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>186.95</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>200.88</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28">
-        <v>164.42</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <v>129.5</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30">
-        <v>154.26</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31">
-        <v>192.39</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
-      <c r="B32">
-        <v>6</v>
-      </c>
-      <c r="C32">
-        <v>2.57</v>
-      </c>
-      <c r="D32">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>3.07</v>
-      </c>
-      <c r="D33">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34">
-        <v>6</v>
-      </c>
-      <c r="C34">
-        <v>2.37</v>
-      </c>
-      <c r="D34">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35">
-        <v>6</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>4</v>
-      </c>
-      <c r="B36">
-        <v>6</v>
-      </c>
-      <c r="C36">
-        <v>1.89</v>
-      </c>
-      <c r="D36">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>2.42</v>
-      </c>
-      <c r="D37">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38">
-        <v>7</v>
-      </c>
-      <c r="C38">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="D38">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39">
-        <v>7</v>
-      </c>
-      <c r="C39">
-        <v>1.92</v>
-      </c>
-      <c r="D39">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40">
-        <v>7</v>
-      </c>
-      <c r="C40">
-        <v>2.09</v>
-      </c>
-      <c r="D40">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>4</v>
-      </c>
-      <c r="B41">
-        <v>7</v>
-      </c>
-      <c r="C41">
-        <v>2.02</v>
-      </c>
-      <c r="D41">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>0</v>
-      </c>
-      <c r="B42">
-        <v>8</v>
-      </c>
-      <c r="C42">
-        <v>0.37</v>
-      </c>
-      <c r="D42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>8</v>
-      </c>
-      <c r="C43">
-        <v>0.24</v>
-      </c>
-      <c r="D43">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2</v>
-      </c>
-      <c r="B44">
-        <v>8</v>
-      </c>
-      <c r="C44">
-        <v>0.22</v>
-      </c>
-      <c r="D44">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>3</v>
-      </c>
-      <c r="B45">
-        <v>8</v>
-      </c>
-      <c r="C45">
-        <v>0.19</v>
-      </c>
-      <c r="D45">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>4</v>
-      </c>
-      <c r="B46">
-        <v>8</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>0</v>
-      </c>
-      <c r="B47">
-        <v>9</v>
-      </c>
-      <c r="C47">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D47">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48">
-        <v>9</v>
-      </c>
-      <c r="C48">
-        <v>0.1</v>
-      </c>
-      <c r="D48">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>2</v>
-      </c>
-      <c r="B49">
-        <v>9</v>
-      </c>
-      <c r="C49">
-        <v>0.1</v>
-      </c>
-      <c r="D49">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>3</v>
-      </c>
-      <c r="B50">
-        <v>9</v>
-      </c>
-      <c r="C50">
-        <v>0.06</v>
-      </c>
-      <c r="D50">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>4</v>
-      </c>
-      <c r="B51">
-        <v>9</v>
-      </c>
-      <c r="C51">
-        <v>0.13</v>
-      </c>
-      <c r="D51">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>0</v>
-      </c>
-      <c r="B52">
-        <v>10</v>
-      </c>
-      <c r="C52">
-        <v>0.19</v>
-      </c>
-      <c r="D52">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53">
-        <v>10</v>
-      </c>
-      <c r="C53">
-        <v>0.26</v>
-      </c>
-      <c r="D53">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>2</v>
-      </c>
-      <c r="B54">
-        <v>10</v>
-      </c>
-      <c r="C54">
-        <v>0.22</v>
-      </c>
-      <c r="D54">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>3</v>
-      </c>
-      <c r="B55">
-        <v>10</v>
-      </c>
-      <c r="C55">
-        <v>0.2</v>
-      </c>
-      <c r="D55">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>4</v>
-      </c>
-      <c r="B56">
-        <v>10</v>
-      </c>
-      <c r="C56">
-        <v>0.23</v>
-      </c>
-      <c r="D56">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>0</v>
-      </c>
-      <c r="B57">
-        <v>11</v>
-      </c>
-      <c r="C57">
-        <v>10.93</v>
-      </c>
-      <c r="D57">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58">
-        <v>11</v>
-      </c>
-      <c r="C58">
-        <v>10.79</v>
-      </c>
-      <c r="D58">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>2</v>
-      </c>
-      <c r="B59">
-        <v>11</v>
-      </c>
-      <c r="C59">
-        <v>10.98</v>
-      </c>
-      <c r="D59">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>3</v>
-      </c>
-      <c r="B60">
-        <v>11</v>
-      </c>
-      <c r="C60">
-        <v>10.71</v>
-      </c>
-      <c r="D60">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>4</v>
-      </c>
-      <c r="B61">
-        <v>11</v>
-      </c>
-      <c r="C61">
-        <v>10.68</v>
-      </c>
-      <c r="D61">
-        <v>3437</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A1:D60">
-    <sortCondition ref="B1:B60"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q55" sqref="Q55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
more detailed analysis of benchmark results
</commit_message>
<xml_diff>
--- a/analysis_lubm100.xlsx
+++ b/analysis_lubm100.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="19155" windowHeight="12465" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="19155" windowHeight="12465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stardog_lubm100" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="10">
   <si>
     <t>iteration</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>timeout</t>
+  </si>
+  <si>
+    <t>distinct issue</t>
+  </si>
+  <si>
+    <t>implicit subclass relationship</t>
   </si>
 </sst>
 </file>
@@ -1652,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,8 +2934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47:G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,7 +3335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3345,8 +3351,11 @@
       <c r="F17" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3362,8 +3371,11 @@
       <c r="F18" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3379,8 +3391,11 @@
       <c r="F19" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3396,8 +3411,11 @@
       <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3413,8 +3431,11 @@
       <c r="F21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -3429,7 +3450,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3444,7 +3465,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -3459,7 +3480,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3474,7 +3495,7 @@
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3489,7 +3510,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -3504,7 +3525,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3519,7 +3540,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -3534,7 +3555,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3549,7 +3570,7 @@
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3564,7 +3585,7 @@
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -3579,7 +3600,7 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3594,7 +3615,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -3609,7 +3630,7 @@
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -3624,7 +3645,7 @@
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3639,7 +3660,7 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0</v>
       </c>
@@ -3655,8 +3676,11 @@
       <c r="F37" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -3672,8 +3696,11 @@
       <c r="F38" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -3689,8 +3716,11 @@
       <c r="F39" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -3706,8 +3736,11 @@
       <c r="F40" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3723,8 +3756,11 @@
       <c r="F41" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -3739,7 +3775,7 @@
       </c>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3754,7 +3790,7 @@
       </c>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -3769,7 +3805,7 @@
       </c>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -3784,7 +3820,7 @@
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -3799,7 +3835,7 @@
       </c>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0</v>
       </c>
@@ -3815,8 +3851,11 @@
       <c r="F47" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3832,8 +3871,11 @@
       <c r="F48" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -3849,8 +3891,11 @@
       <c r="F49" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -3866,8 +3911,11 @@
       <c r="F50" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -3883,8 +3931,11 @@
       <c r="F51" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -3899,7 +3950,7 @@
       </c>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -3914,7 +3965,7 @@
       </c>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3929,7 +3980,7 @@
       </c>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -3944,7 +3995,7 @@
       </c>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -3959,7 +4010,7 @@
       </c>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0</v>
       </c>
@@ -3976,7 +4027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -3993,7 +4044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -4010,7 +4061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -4027,7 +4078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -4044,7 +4095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0</v>
       </c>
@@ -4059,7 +4110,7 @@
       </c>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1</v>
       </c>
@@ -4074,7 +4125,7 @@
       </c>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4206,7 +4257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>

</xml_diff>